<commit_message>
Book excel half update
</commit_message>
<xml_diff>
--- a/Doc/book.xlsx
+++ b/Doc/book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VICTUS\OneDrive\Desktop\Normal softwer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\LibraryManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0268D2-D584-47FB-B36F-2790F07D3159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB3BDB0-E04D-460B-931C-831B2ED4AE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5DB3DE8-FD8F-4413-849B-11553E2EF562}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8E09630E-FBB8-4CD5-98D8-40C1A54718B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,19 +35,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>NUM1</t>
-  </si>
-  <si>
-    <t>NUM2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Book No</t>
+  </si>
+  <si>
+    <t>Author 1</t>
+  </si>
+  <si>
+    <t>Author 2</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Edition</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>CL Number</t>
+  </si>
+  <si>
+    <t>Total Pages</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>Bill_No</t>
+  </si>
+  <si>
+    <t>holly cow</t>
+  </si>
+  <si>
+    <t>hijfds</t>
+  </si>
+  <si>
+    <t>hghvfhjg</t>
+  </si>
+  <si>
+    <t>hjkgkgvhjgk</t>
+  </si>
+  <si>
+    <t>hj,vbhjkg</t>
+  </si>
+  <si>
+    <t>hv,bjhjk</t>
+  </si>
+  <si>
+    <t>jkkhg</t>
+  </si>
+  <si>
+    <t>hjkgkhjgvgj</t>
+  </si>
+  <si>
+    <t>jkhv</t>
+  </si>
+  <si>
+    <t>Title 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,13 +115,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,8 +149,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,40 +468,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30CCBD73-F258-4C15-B617-26A3594D5081}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E477230-9697-4CD6-924B-FB7D80C68E81}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>6.4</v>
+      </c>
+      <c r="I2">
+        <v>97</v>
+      </c>
+      <c r="J2">
+        <v>351</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>